<commit_message>
report table adjustment,  excel template adjustmen
Co-Authored-By: meira <212976802+merazea@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/docs/Employee_Record_Template.xlsx
+++ b/docs/Employee_Record_Template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olalekan\Desktop\jfiles\payroll\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daffa\Git Repository\OnPayroll-app\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED086EE8-BBD7-454F-8BFC-B22CBFA0A106}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{494C47C6-4205-4472-B4B1-F125E89BF183}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{46D5286B-7FCC-4DF1-83F0-20D39316EDCA}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>name</t>
   </si>
@@ -54,13 +54,22 @@
     <t>accountNumber</t>
   </si>
   <si>
-    <t>pfaName</t>
-  </si>
-  <si>
-    <t>pensionAccountNumber</t>
-  </si>
-  <si>
     <t>levelName</t>
+  </si>
+  <si>
+    <t>gender</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>bpjsKetenagakerjaanNumber</t>
+  </si>
+  <si>
+    <t>bpjsKesehatanNumber</t>
+  </si>
+  <si>
+    <t>npwp</t>
   </si>
 </sst>
 </file>
@@ -432,10 +441,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AA0EF98-512A-4FE7-9A2D-5954A090D613}">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="P6" sqref="P6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -449,42 +458,54 @@
     <col min="7" max="7" width="21.85546875" customWidth="1"/>
     <col min="8" max="8" width="19.5703125" customWidth="1"/>
     <col min="9" max="9" width="24.140625" customWidth="1"/>
-    <col min="10" max="10" width="17.28515625" customWidth="1"/>
+    <col min="10" max="10" width="30.85546875" customWidth="1"/>
+    <col min="11" max="11" width="27" customWidth="1"/>
+    <col min="12" max="12" width="17.28515625" customWidth="1"/>
+    <col min="13" max="13" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="J1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>9</v>
-      </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B2" s="1"/>
     </row>
   </sheetData>

</xml_diff>